<commit_message>
version to compare two types of layout
</commit_message>
<xml_diff>
--- a/thesis_doc/collaborators/althea/table1_idea20181101.xlsx
+++ b/thesis_doc/collaborators/althea/table1_idea20181101.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/althea/Documents/professional/mentoring/2017/edwards_magaret/thesis/thesis/thesis_doc/collaborators/althea/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DE84286-04C7-BC40-9E8D-79DA67C94CDC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A594A91-F128-D246-B6D9-4A1EB024696E}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="960" yWindow="440" windowWidth="24560" windowHeight="15020" xr2:uid="{A62F97A2-F06D-FD4F-BE46-2B2032DAAB35}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="56">
   <si>
     <t>Dynamics</t>
   </si>
@@ -163,6 +163,36 @@
   </si>
   <si>
     <t>Detection Models</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>Abundance Model</t>
+  </si>
+  <si>
+    <t>Detection Model</t>
+  </si>
+  <si>
+    <t>B0lambda</t>
+  </si>
+  <si>
+    <t>B1lambda</t>
+  </si>
+  <si>
+    <t>B0p</t>
+  </si>
+  <si>
+    <t>B1p</t>
+  </si>
+  <si>
+    <t>B2p</t>
+  </si>
+  <si>
+    <t>Null</t>
+  </si>
+  <si>
+    <t>Multiple</t>
   </si>
 </sst>
 </file>
@@ -199,7 +229,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -225,11 +255,29 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -258,6 +306,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -267,7 +319,56 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,25 +686,44 @@
   <dimension ref="A1:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="L14" sqref="L14:Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12"/>
-      <c r="F1" s="12"/>
-      <c r="G1" s="13" t="s">
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="I1" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="M1" s="24"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
@@ -622,7 +742,30 @@
       <c r="F2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="16"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="K2" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="M2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="N2" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q2" s="20"/>
     </row>
     <row r="3" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -643,7 +786,36 @@
       <c r="F3" s="2">
         <v>0.26</v>
       </c>
-      <c r="G3" s="2"/>
+      <c r="G3" s="2">
+        <v>-2.97</v>
+      </c>
+      <c r="I3" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="18">
+        <v>-2.97</v>
+      </c>
+      <c r="K3" s="22">
+        <v>4.13</v>
+      </c>
+      <c r="L3" s="18">
+        <v>-1.85</v>
+      </c>
+      <c r="M3" s="22">
+        <v>0.26</v>
+      </c>
+      <c r="N3" s="22">
+        <v>0.33</v>
+      </c>
+      <c r="O3" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="P3" s="18">
+        <v>-2.25</v>
+      </c>
+      <c r="Q3" s="24">
+        <v>442.73</v>
+      </c>
     </row>
     <row r="4" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="8"/>
@@ -662,15 +834,32 @@
       <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="J4" s="1"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
+      <c r="G4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="25"/>
+      <c r="J4" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="K4" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="L4" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="O4" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="P4" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q4" s="27"/>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -692,10 +881,36 @@
       <c r="F5" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="J5" s="1"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
+      <c r="G5" s="3">
+        <v>4.13</v>
+      </c>
+      <c r="I5" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="18">
+        <v>-7.0000000000000007E-2</v>
+      </c>
+      <c r="K5" s="22">
+        <v>-0.85</v>
+      </c>
+      <c r="L5" s="18">
+        <v>-1.7</v>
+      </c>
+      <c r="M5" s="18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N5" s="22">
+        <v>0.36</v>
+      </c>
+      <c r="O5" s="18">
+        <v>0.27</v>
+      </c>
+      <c r="P5" s="18">
+        <v>-2.16</v>
+      </c>
+      <c r="Q5" s="27">
+        <v>461.61</v>
+      </c>
       <c r="R5" s="2"/>
     </row>
     <row r="6" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -715,10 +930,32 @@
       <c r="F6" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="J6" s="1"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="25"/>
+      <c r="J6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="L6" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="M6" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="O6" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q6" s="27"/>
       <c r="R6" s="2"/>
     </row>
     <row r="7" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -740,8 +977,36 @@
       <c r="F7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="J7" s="1"/>
+      <c r="G7" s="3">
+        <v>-0.85</v>
+      </c>
+      <c r="I7" s="25" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="18">
+        <v>0.13</v>
+      </c>
+      <c r="K7" s="22">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="L7" s="18">
+        <v>-1.78</v>
+      </c>
+      <c r="M7" s="22">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N7" s="22">
+        <v>0.37</v>
+      </c>
+      <c r="O7" s="18">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="P7" s="18">
+        <v>-2.12</v>
+      </c>
+      <c r="Q7" s="27">
+        <v>463.78</v>
+      </c>
       <c r="R7" s="2"/>
     </row>
     <row r="8" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -761,8 +1026,32 @@
       <c r="F8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="J8" s="1"/>
+      <c r="G8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="25"/>
+      <c r="J8" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="K8" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="L8" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="O8" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="P8" s="18" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q8" s="27"/>
       <c r="R8" s="2"/>
     </row>
     <row r="9" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -784,8 +1073,36 @@
       <c r="F9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="J9" s="1"/>
+      <c r="G9" s="3">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>54</v>
+      </c>
+      <c r="J9" s="18">
+        <v>0.26</v>
+      </c>
+      <c r="K9" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L9" s="18">
+        <v>-1.74</v>
+      </c>
+      <c r="M9" s="22">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N9" s="22">
+        <v>0.37</v>
+      </c>
+      <c r="O9" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="P9" s="18">
+        <v>-2.09</v>
+      </c>
+      <c r="Q9" s="27">
+        <v>464.09</v>
+      </c>
       <c r="R9" s="2"/>
     </row>
     <row r="10" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -805,8 +1122,32 @@
       <c r="F10" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="J10" s="1"/>
+      <c r="G10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="25"/>
+      <c r="J10" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="L10" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="O10" s="18" t="s">
+        <v>29</v>
+      </c>
+      <c r="P10" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q10" s="27"/>
       <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -831,11 +1172,36 @@
       <c r="G11" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="1"/>
-      <c r="L11" s="2"/>
+      <c r="I11" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="18">
+        <v>0.26</v>
+      </c>
+      <c r="K11" s="18">
+        <v>-0.01</v>
+      </c>
+      <c r="L11" s="18">
+        <v>-1.74</v>
+      </c>
+      <c r="M11" s="22">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="N11" s="22">
+        <v>0.37</v>
+      </c>
+      <c r="O11" s="18">
+        <v>0.03</v>
+      </c>
+      <c r="P11" s="18">
+        <v>-2.09</v>
+      </c>
+      <c r="Q11" s="27">
+        <v>466.09</v>
+      </c>
       <c r="R11" s="2"/>
     </row>
-    <row r="12" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="19" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="2" t="s">
         <v>27</v>
@@ -855,20 +1221,44 @@
       <c r="G12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="1"/>
-      <c r="L12" s="2"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K12" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="M12" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q12" s="29"/>
       <c r="R12" s="2"/>
     </row>
     <row r="13" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="12" t="s">
+      <c r="A13" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="I13" t="s">
+        <v>55</v>
+      </c>
       <c r="J13" s="1"/>
       <c r="L13" s="2"/>
       <c r="R13" s="2"/>
@@ -892,8 +1282,36 @@
       <c r="F14" s="2">
         <v>-1.74</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="J14" s="1"/>
+      <c r="G14" s="2">
+        <v>-1.85</v>
+      </c>
+      <c r="I14" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="J14" s="18">
+        <v>-2.97</v>
+      </c>
+      <c r="K14" s="22">
+        <v>4.13</v>
+      </c>
+      <c r="L14" s="18">
+        <v>-1.85</v>
+      </c>
+      <c r="M14" s="22">
+        <v>0.26</v>
+      </c>
+      <c r="N14" s="22">
+        <v>0.33</v>
+      </c>
+      <c r="O14" s="18">
+        <v>0.25</v>
+      </c>
+      <c r="P14" s="18">
+        <v>-2.25</v>
+      </c>
+      <c r="Q14" s="34">
+        <v>442.73</v>
+      </c>
       <c r="R14" s="2"/>
     </row>
     <row r="15" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -913,8 +1331,32 @@
       <c r="F15" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="J15" s="1"/>
+      <c r="G15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="25"/>
+      <c r="J15" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="K15" s="22" t="s">
+        <v>6</v>
+      </c>
+      <c r="L15" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="M15" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="N15" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="O15" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="P15" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q15" s="34"/>
       <c r="R15" s="2"/>
     </row>
     <row r="16" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.2">
@@ -936,9 +1378,17 @@
       <c r="F16" s="3">
         <v>0.28999999999999998</v>
       </c>
-      <c r="G16" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G16" s="3">
+        <v>0.26</v>
+      </c>
+      <c r="I16" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="22">
+        <v>-0.85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="3" t="s">
         <v>8</v>
@@ -955,9 +1405,15 @@
       <c r="F17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G17" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I17" s="25"/>
+      <c r="K17" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>37</v>
       </c>
@@ -976,9 +1432,24 @@
       <c r="F18" s="3">
         <v>0.37</v>
       </c>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G18" s="3">
+        <v>0.33</v>
+      </c>
+      <c r="I18" s="30" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18" s="31"/>
+      <c r="K18" s="3">
+        <v>-0.57999999999999996</v>
+      </c>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+    </row>
+    <row r="19" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="3" t="s">
         <v>9</v>
@@ -995,9 +1466,22 @@
       <c r="F19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G19" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I19" s="32"/>
+      <c r="J19" s="33"/>
+      <c r="K19" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="L19" s="33"/>
+      <c r="M19" s="33"/>
+      <c r="N19" s="33"/>
+      <c r="O19" s="33"/>
+      <c r="P19" s="33"/>
+      <c r="Q19" s="33"/>
+    </row>
+    <row r="20" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>0</v>
       </c>
@@ -1008,7 +1492,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="9"/>
     </row>
-    <row r="21" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="8" t="s">
         <v>2</v>
       </c>
@@ -1027,9 +1511,11 @@
       <c r="F21" s="2">
         <v>0.03</v>
       </c>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G21" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
         <v>10</v>
@@ -1046,9 +1532,11 @@
       <c r="F22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>3</v>
       </c>
@@ -1067,9 +1555,11 @@
       <c r="F23" s="2">
         <v>-2.09</v>
       </c>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="G23" s="2">
+        <v>-2.25</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="6" t="s">
         <v>11</v>
@@ -1086,10 +1576,12 @@
       <c r="F24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="1:7" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
+      <c r="G24" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" ht="19" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B25" s="6">
@@ -1107,13 +1599,32 @@
       <c r="F25" s="6">
         <v>466.09</v>
       </c>
-      <c r="G25" s="10"/>
+      <c r="G25" s="6">
+        <v>442.73</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="20">
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="I16:I17"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="Q14:Q15"/>
+    <mergeCell ref="Q7:Q8"/>
+    <mergeCell ref="I9:I10"/>
+    <mergeCell ref="Q9:Q10"/>
+    <mergeCell ref="I11:I12"/>
+    <mergeCell ref="Q11:Q12"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="Q3:Q4"/>
+    <mergeCell ref="I5:I6"/>
+    <mergeCell ref="Q5:Q6"/>
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A13:G13"/>
     <mergeCell ref="G1:G2"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="I7:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>